<commit_message>
renamed variables and manually did cardinality graph
</commit_message>
<xml_diff>
--- a/dataset/final_dataset.xlsx
+++ b/dataset/final_dataset.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -441,37 +441,37 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>genderratio</t>
+          <t>Gender Ratio</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>nationalitymix</t>
+          <t>Minority Ratio</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>voting_power</t>
+          <t>VotePower</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>percentage_INEDs</t>
+          <t>%INEDS</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>num_directors_&gt;4.5</t>
+          <t>Number Directors'Own&gt;4.5</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>total_share_%</t>
+          <t>Board Ownership</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>boardsize</t>
+          <t>Board Size</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -481,12 +481,12 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>CEODuality</t>
+          <t>CEO Dual</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>dualclass</t>
+          <t>Dualclass Voting</t>
         </is>
       </c>
     </row>
@@ -10080,10 +10080,10 @@
         </is>
       </c>
       <c r="B261" t="n">
-        <v>0.6920000000000001</v>
+        <v>0.636</v>
       </c>
       <c r="C261" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="D261" t="n">
         <v>46.2</v>

</xml_diff>